<commit_message>
changes before trying new option with new branch
</commit_message>
<xml_diff>
--- a/Test Output Garbage Dump/HI-CRISPR Knockout/The Mega 100 Gene Knockout.xlsx
+++ b/Test Output Garbage Dump/HI-CRISPR Knockout/The Mega 100 Gene Knockout.xlsx
@@ -495,7 +495,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GCCCTAATCTAACCCTGGCC</t>
+          <t>TACCCTGCCTCCACTCGTTA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GTAAGTGGCAGTGGGTTGGA</t>
+          <t>AGTATGGCATGTGGTGGTGG</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">

</xml_diff>